<commit_message>
generation and zones clustrering
</commit_message>
<xml_diff>
--- a/inputs/parameters.xlsx
+++ b/inputs/parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
   <si>
     <t xml:space="preserve">Fichier de paramètre du modèle Quetzal Montréal</t>
   </si>
@@ -351,6 +351,87 @@
   <si>
     <t xml:space="preserve">road_to_transit speed (acf)</t>
   </si>
+  <si>
+    <t xml:space="preserve">logit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût kilométrique de la voiture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waiting_time_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facteur de perception du temp d'attente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walking_time_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facteur de perception du temp de marche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preparation_logit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur utilitaire du temps (Pour le calcul du facteur multiplication du temps de la fonction d'utilité)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min/pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur monétaire du temps (Pour le calcul du facteur multiplication du coût de la fonction d'utilité)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$/hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facteur multiplicatif de l'utilité associé au mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pt_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient du logit des modes PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pt_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient du logit du nœud PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient de pénalité de transfert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min/transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step_distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taux de motorisation</t>
+  </si>
 </sst>
 </file>
 
@@ -359,7 +440,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,12 +493,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -503,7 +578,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,8 +655,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -836,8 +919,8 @@
     <mergeCell ref="A2:B4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -855,7 +938,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topRight" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -864,7 +947,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="41.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="34"/>
@@ -1611,6 +1694,195 @@
       </c>
       <c r="H9" s="18"/>
     </row>
+    <row r="10" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="0"/>
+      <c r="G10" s="21" t="n">
+        <v>0.00032</v>
+      </c>
+      <c r="H10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="21" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="21" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="0"/>
+      <c r="G13" s="21" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="0"/>
+      <c r="G14" s="21" t="n">
+        <v>15</v>
+      </c>
+      <c r="H14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="0"/>
+      <c r="G18" s="21" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1672,8 +1944,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
pathfinder with broken mode
</commit_message>
<xml_diff>
--- a/inputs/parameters.xlsx
+++ b/inputs/parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t xml:space="preserve">Fichier de paramètre du modèle Quetzal Montréal</t>
   </si>
@@ -352,6 +352,21 @@
     <t xml:space="preserve">road_to_transit speed (acf)</t>
   </si>
   <si>
+    <t xml:space="preserve">pathfinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode_breaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longueur maximale des autres itinéraires PT</t>
+  </si>
+  <si>
     <t xml:space="preserve">logit</t>
   </si>
   <si>
@@ -437,8 +452,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -578,7 +594,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,6 +673,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -919,8 +943,8 @@
     <mergeCell ref="A2:B4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -938,7 +962,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topRight" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1694,195 +1718,224 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+    <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20" t="s">
+      <c r="F10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="G10" s="20" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="0"/>
-      <c r="G10" s="21" t="n">
+      <c r="D11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="0"/>
+      <c r="G12" s="23" t="n">
         <v>0.00032</v>
       </c>
-      <c r="H10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="20" t="s">
+      <c r="H12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="21" t="n">
+      <c r="B13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="23" t="n">
         <v>1.6</v>
       </c>
-      <c r="H11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="21" t="n">
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="23" t="n">
         <v>1.3</v>
       </c>
-      <c r="H12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="0"/>
-      <c r="G13" s="21" t="n">
+      <c r="H14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="0"/>
+      <c r="G15" s="23" t="n">
         <v>20</v>
       </c>
-      <c r="H13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20" t="s">
+      <c r="H15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="0"/>
-      <c r="G14" s="21" t="n">
+      <c r="B16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="0"/>
+      <c r="G16" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="H14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="21" t="n">
-        <v>0.5</v>
-      </c>
       <c r="H16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>74</v>
+      <c r="A17" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="20" t="s">
-        <v>75</v>
+      <c r="D17" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="21" t="n">
+      <c r="G17" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="23" t="n">
         <v>0.1</v>
       </c>
-      <c r="H17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="0"/>
-      <c r="G18" s="21" t="n">
+      <c r="H19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="0"/>
+      <c r="G20" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="H18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="H20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="12" t="n">
+      <c r="G21" s="12" t="n">
         <v>0.8</v>
       </c>
     </row>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1935,7 +1988,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="H3:H9">
+  <conditionalFormatting sqref="H3:H11">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>_xlfn.ISFORMULA(#ref!)</formula>
     </cfRule>
@@ -1944,8 +1997,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>